<commit_message>
added Dockerfile and functions for simulating exceeded projects
</commit_message>
<xml_diff>
--- a/delphin_6_automation/sampling/input_files/Natural Stone.xlsx
+++ b/delphin_6_automation/sampling/input_files/Natural Stone.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Material ID</t>
   </si>
@@ -97,6 +97,30 @@
   </si>
   <si>
     <t>WeatheredGranite</t>
+  </si>
+  <si>
+    <t>limesandstone</t>
+  </si>
+  <si>
+    <t>LimeSandBrick</t>
+  </si>
+  <si>
+    <t>XellaKalksandstein</t>
+  </si>
+  <si>
+    <t>KalksandsteinXellaYtong2002</t>
+  </si>
+  <si>
+    <t>KalksandsteinXellaYtong2004</t>
+  </si>
+  <si>
+    <t>LimeSandbrick</t>
+  </si>
+  <si>
+    <t>LimeSandBrickTraditional</t>
+  </si>
+  <si>
+    <t>LimeSandBrickIndustrial</t>
   </si>
 </sst>
 </file>
@@ -149,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,6 +181,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,208 +486,272 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>219</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="A2" s="3">
+        <v>152</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>220</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+      <c r="A3" s="3">
+        <v>153</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>263</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>461</v>
+        <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>462</v>
+        <v>263</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>558</v>
+        <v>471</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>559</v>
+        <v>472</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>561</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
+      <c r="A19" s="3">
+        <v>509</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>562</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
+      <c r="A20" s="3">
+        <v>510</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>563</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
+      <c r="A21" s="3">
+        <v>511</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>564</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
+      <c r="A22" s="3">
+        <v>550</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>565</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
+      <c r="A23" s="3">
+        <v>551</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
+        <v>561</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>562</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>563</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>564</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>565</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>566</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>567</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>568</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B33" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>685</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:B26">
-    <sortCondition ref="A2:A26"/>
+  <sortState ref="A2:B34">
+    <sortCondition ref="A2:A34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>